<commit_message>
re-compute average S-map coefficient of abundance
</commit_message>
<xml_diff>
--- a/output/smap/Smap_abundance_coefficients_vs_b.xlsx
+++ b/output/smap/Smap_abundance_coefficients_vs_b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -431,16 +431,16 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G2" sqref="G2:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.25" customWidth="1"/>
-    <col min="2" max="2" width="7.875" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -460,7 +460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,7 +500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -520,7 +520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -528,10 +528,10 @@
         <v>1.9622999999999999</v>
       </c>
       <c r="C5">
-        <v>-0.42920000000000003</v>
+        <v>-0.51800000000000002</v>
       </c>
       <c r="D5">
-        <v>0.15</v>
+        <v>0.29659999999999997</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -540,7 +540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -560,7 +560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -568,10 +568,10 @@
         <v>2.1585999999999999</v>
       </c>
       <c r="C7">
-        <v>0.3085</v>
+        <v>0.34189999999999998</v>
       </c>
       <c r="D7">
-        <v>0.27</v>
+        <v>0.1978</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -580,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -600,7 +600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -620,7 +620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>